<commit_message>
changed dataset prepare code to process data collected from real people completed multiple input recommender syystem
</commit_message>
<xml_diff>
--- a/05180000017_Deniz_Yürekdeler_Project2/ActivityRecommender_PythonCode/Real-Data/Activity-Rating-Real-Data.xlsx
+++ b/05180000017_Deniz_Yürekdeler_Project2/ActivityRecommender_PythonCode/Real-Data/Activity-Rating-Real-Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>activityId</t>
   </si>
@@ -128,9 +128,6 @@
     <t>eating-outside</t>
   </si>
   <si>
-    <t>eating-dinner</t>
-  </si>
-  <si>
     <t>eating-dessert</t>
   </si>
   <si>
@@ -201,19 +198,78 @@
   </si>
   <si>
     <t>Can</t>
+  </si>
+  <si>
+    <t>playing-football</t>
+  </si>
+  <si>
+    <t>playing-basketball</t>
+  </si>
+  <si>
+    <t>playing-volleyball</t>
+  </si>
+  <si>
+    <t>meeting-family</t>
+  </si>
+  <si>
+    <t>visiting-beach</t>
+  </si>
+  <si>
+    <t>Mustafa</t>
+  </si>
+  <si>
+    <t>Civan</t>
+  </si>
+  <si>
+    <t>Abdullah</t>
+  </si>
+  <si>
+    <t>Dilara</t>
+  </si>
+  <si>
+    <t>Deniz</t>
+  </si>
+  <si>
+    <t>Rasit</t>
+  </si>
+  <si>
+    <t>Ulku</t>
+  </si>
+  <si>
+    <t>Dogukan</t>
+  </si>
+  <si>
+    <t>Kaan</t>
+  </si>
+  <si>
+    <t>KaanGircek</t>
+  </si>
+  <si>
+    <t>Omer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -233,15 +289,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -519,19 +592,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,19 +613,52 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>1</v>
       </c>
@@ -567,8 +674,44 @@
       <c r="E2" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2">
+        <v>5</v>
+      </c>
+      <c r="K2" s="2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>2</v>
       </c>
@@ -584,8 +727,44 @@
       <c r="E3" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>3</v>
       </c>
@@ -601,8 +780,44 @@
       <c r="E4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>4</v>
       </c>
@@ -618,8 +833,44 @@
       <c r="E5" s="1">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>5</v>
       </c>
@@ -635,8 +886,44 @@
       <c r="E6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>6</v>
       </c>
@@ -652,8 +939,44 @@
       <c r="E7" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>5</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>4.5</v>
+      </c>
+      <c r="P7" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>7</v>
       </c>
@@ -669,8 +992,44 @@
       <c r="E8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>4.5</v>
+      </c>
+      <c r="P8" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>8</v>
       </c>
@@ -686,8 +1045,44 @@
       <c r="E9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>3</v>
+      </c>
+      <c r="P9" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>9</v>
       </c>
@@ -703,8 +1098,44 @@
       <c r="E10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>3.5</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>3</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>10</v>
       </c>
@@ -720,8 +1151,44 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>3.5</v>
+      </c>
+      <c r="P11" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>11</v>
       </c>
@@ -737,8 +1204,44 @@
       <c r="E12" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
+      <c r="K12" s="2">
+        <v>5</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
+      <c r="P12" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>12</v>
       </c>
@@ -754,8 +1257,44 @@
       <c r="E13" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>3.5</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13" s="2">
+        <v>5</v>
+      </c>
+      <c r="J13" s="2">
+        <v>5</v>
+      </c>
+      <c r="K13" s="2">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+      <c r="P13" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>13</v>
       </c>
@@ -771,8 +1310,44 @@
       <c r="E14" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14" s="2">
+        <v>5</v>
+      </c>
+      <c r="J14" s="2">
+        <v>4</v>
+      </c>
+      <c r="K14" s="2">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>5</v>
+      </c>
+      <c r="M14">
+        <v>5</v>
+      </c>
+      <c r="N14">
+        <v>4</v>
+      </c>
+      <c r="O14">
+        <v>5</v>
+      </c>
+      <c r="P14" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>14</v>
       </c>
@@ -788,8 +1363,44 @@
       <c r="E15" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="1">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15" s="2">
+        <v>5</v>
+      </c>
+      <c r="J15" s="2">
+        <v>4</v>
+      </c>
+      <c r="K15" s="2">
+        <v>5</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <v>4</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="P15" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>15</v>
       </c>
@@ -805,8 +1416,44 @@
       <c r="E16" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16" s="2">
+        <v>3</v>
+      </c>
+      <c r="J16" s="2">
+        <v>4</v>
+      </c>
+      <c r="K16" s="2">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>5</v>
+      </c>
+      <c r="P16" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>16</v>
       </c>
@@ -822,8 +1469,44 @@
       <c r="E17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>3</v>
+      </c>
+      <c r="K17" s="2">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>3</v>
+      </c>
+      <c r="O17">
+        <v>5</v>
+      </c>
+      <c r="P17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>17</v>
       </c>
@@ -839,8 +1522,44 @@
       <c r="E18" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2">
+        <v>2</v>
+      </c>
+      <c r="K18" s="2">
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>18</v>
       </c>
@@ -856,8 +1575,44 @@
       <c r="E19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="1">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19" s="2">
+        <v>2</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <v>5</v>
+      </c>
+      <c r="M19">
+        <v>5</v>
+      </c>
+      <c r="N19">
+        <v>4</v>
+      </c>
+      <c r="O19">
+        <v>3.5</v>
+      </c>
+      <c r="P19" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>19</v>
       </c>
@@ -873,8 +1628,44 @@
       <c r="E20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2">
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <v>5</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+      <c r="O20">
+        <v>3</v>
+      </c>
+      <c r="P20" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>20</v>
       </c>
@@ -890,8 +1681,44 @@
       <c r="E21" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="1">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21" s="2">
+        <v>2</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1</v>
+      </c>
+      <c r="K21" s="2">
+        <v>5</v>
+      </c>
+      <c r="L21">
+        <v>4</v>
+      </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
+      <c r="N21">
+        <v>4</v>
+      </c>
+      <c r="O21">
+        <v>4</v>
+      </c>
+      <c r="P21" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>21</v>
       </c>
@@ -907,8 +1734,44 @@
       <c r="E22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>5</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
+      <c r="N22">
+        <v>3</v>
+      </c>
+      <c r="O22">
+        <v>2</v>
+      </c>
+      <c r="P22" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>22</v>
       </c>
@@ -924,8 +1787,44 @@
       <c r="E23" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="1">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23" s="2">
+        <v>3</v>
+      </c>
+      <c r="J23" s="2">
+        <v>3</v>
+      </c>
+      <c r="K23" s="2">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <v>3</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>4</v>
+      </c>
+      <c r="O23">
+        <v>3.5</v>
+      </c>
+      <c r="P23" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>23</v>
       </c>
@@ -941,8 +1840,44 @@
       <c r="E24" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24" s="2">
+        <v>2</v>
+      </c>
+      <c r="J24" s="2">
+        <v>4</v>
+      </c>
+      <c r="K24" s="2">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+      <c r="O24">
+        <v>5</v>
+      </c>
+      <c r="P24" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25">
         <v>24</v>
       </c>
@@ -958,8 +1893,44 @@
       <c r="E25" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="1">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+      <c r="I25" s="2">
+        <v>4</v>
+      </c>
+      <c r="J25" s="2">
+        <v>5</v>
+      </c>
+      <c r="K25" s="2">
+        <v>5</v>
+      </c>
+      <c r="L25">
+        <v>5</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <v>4</v>
+      </c>
+      <c r="O25">
+        <v>5</v>
+      </c>
+      <c r="P25" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26">
         <v>25</v>
       </c>
@@ -975,8 +1946,44 @@
       <c r="E26" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>3.5</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26" s="2">
+        <v>2</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>4</v>
+      </c>
+      <c r="M26">
+        <v>2</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>26</v>
       </c>
@@ -992,8 +1999,44 @@
       <c r="E27" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2">
+        <v>4</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <v>3</v>
+      </c>
+      <c r="M27">
+        <v>5</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>4</v>
+      </c>
+      <c r="P27" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1009,8 +2052,44 @@
       <c r="E28" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28" s="2">
+        <v>5</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>5</v>
+      </c>
+      <c r="M28">
+        <v>5</v>
+      </c>
+      <c r="N28">
+        <v>3</v>
+      </c>
+      <c r="O28">
+        <v>4</v>
+      </c>
+      <c r="P28" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1026,8 +2105,44 @@
       <c r="E29" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29" s="2">
+        <v>3</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2">
+        <v>5</v>
+      </c>
+      <c r="L29">
+        <v>3</v>
+      </c>
+      <c r="M29">
+        <v>5</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1043,8 +2158,44 @@
       <c r="E30" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2">
+        <v>5</v>
+      </c>
+      <c r="L30">
+        <v>3</v>
+      </c>
+      <c r="M30">
+        <v>4</v>
+      </c>
+      <c r="N30">
+        <v>4</v>
+      </c>
+      <c r="O30">
+        <v>5</v>
+      </c>
+      <c r="P30" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1060,8 +2211,44 @@
       <c r="E31" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="1">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31" s="2">
+        <v>4</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2">
+        <v>5</v>
+      </c>
+      <c r="L31">
+        <v>4</v>
+      </c>
+      <c r="M31">
+        <v>5</v>
+      </c>
+      <c r="N31">
+        <v>4</v>
+      </c>
+      <c r="O31">
+        <v>5</v>
+      </c>
+      <c r="P31" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1077,8 +2264,44 @@
       <c r="E32" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>3.5</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32" s="2">
+        <v>3</v>
+      </c>
+      <c r="J32" s="2">
+        <v>5</v>
+      </c>
+      <c r="K32" s="2">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>5</v>
+      </c>
+      <c r="M32">
+        <v>5</v>
+      </c>
+      <c r="N32">
+        <v>4</v>
+      </c>
+      <c r="O32">
+        <v>5</v>
+      </c>
+      <c r="P32" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1094,8 +2317,44 @@
       <c r="E33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="1">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>2.5</v>
+      </c>
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="I33" s="2">
+        <v>4</v>
+      </c>
+      <c r="J33" s="2">
+        <v>4</v>
+      </c>
+      <c r="K33" s="2">
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
+      <c r="M33">
+        <v>3</v>
+      </c>
+      <c r="N33">
+        <v>4</v>
+      </c>
+      <c r="O33">
+        <v>5</v>
+      </c>
+      <c r="P33" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1109,10 +2368,46 @@
         <v>5</v>
       </c>
       <c r="E34" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <v>4</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34" s="2">
+        <v>3</v>
+      </c>
+      <c r="J34" s="2">
+        <v>4</v>
+      </c>
+      <c r="K34" s="2">
+        <v>3</v>
+      </c>
+      <c r="L34">
+        <v>2</v>
+      </c>
+      <c r="M34">
+        <v>5</v>
+      </c>
+      <c r="N34">
+        <v>4</v>
+      </c>
+      <c r="O34">
+        <v>5</v>
+      </c>
+      <c r="P34" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1120,7 +2415,7 @@
         <v>35</v>
       </c>
       <c r="C35">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D35" s="1">
         <v>5</v>
@@ -1128,8 +2423,44 @@
       <c r="E35" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="1">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35" s="2">
+        <v>3</v>
+      </c>
+      <c r="J35" s="2">
+        <v>4</v>
+      </c>
+      <c r="K35" s="2">
+        <v>3</v>
+      </c>
+      <c r="L35">
+        <v>3</v>
+      </c>
+      <c r="M35">
+        <v>4</v>
+      </c>
+      <c r="N35">
+        <v>4</v>
+      </c>
+      <c r="O35">
+        <v>5</v>
+      </c>
+      <c r="P35" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1137,16 +2468,52 @@
         <v>36</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D36" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36" s="2">
+        <v>1</v>
+      </c>
+      <c r="J36" s="2">
+        <v>4</v>
+      </c>
+      <c r="K36" s="2">
+        <v>2</v>
+      </c>
+      <c r="L36">
+        <v>5</v>
+      </c>
+      <c r="M36">
+        <v>5</v>
+      </c>
+      <c r="N36">
+        <v>4</v>
+      </c>
+      <c r="O36">
+        <v>3.5</v>
+      </c>
+      <c r="P36" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1154,16 +2521,52 @@
         <v>37</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>3</v>
+      </c>
+      <c r="I37" s="2">
+        <v>5</v>
+      </c>
+      <c r="J37" s="2">
+        <v>4</v>
+      </c>
+      <c r="K37" s="2">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>4</v>
+      </c>
+      <c r="M37">
+        <v>4</v>
+      </c>
+      <c r="N37">
+        <v>4</v>
+      </c>
+      <c r="O37">
+        <v>5</v>
+      </c>
+      <c r="P37" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1171,16 +2574,52 @@
         <v>38</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F38" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G38">
+        <v>2.5</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38" s="2">
+        <v>4</v>
+      </c>
+      <c r="J38" s="2">
+        <v>4</v>
+      </c>
+      <c r="K38" s="2">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>3</v>
+      </c>
+      <c r="M38">
+        <v>2</v>
+      </c>
+      <c r="N38">
+        <v>2</v>
+      </c>
+      <c r="O38">
+        <v>4</v>
+      </c>
+      <c r="P38" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1188,16 +2627,52 @@
         <v>39</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="1">
         <v>3</v>
       </c>
       <c r="E39" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+      <c r="F39" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+      <c r="I39" s="2">
+        <v>4</v>
+      </c>
+      <c r="J39" s="2">
+        <v>4</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>2</v>
+      </c>
+      <c r="N39">
+        <v>3</v>
+      </c>
+      <c r="O39">
+        <v>3.5</v>
+      </c>
+      <c r="P39" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1205,16 +2680,52 @@
         <v>40</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D40" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E40" s="1">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F40" s="1">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>5</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40" s="2">
+        <v>4</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0</v>
+      </c>
+      <c r="K40" s="2">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>4</v>
+      </c>
+      <c r="M40">
+        <v>3</v>
+      </c>
+      <c r="N40">
+        <v>3</v>
+      </c>
+      <c r="O40">
+        <v>3.5</v>
+      </c>
+      <c r="P40" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q40" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1222,16 +2733,52 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D41" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E41" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F41" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41" s="2">
+        <v>0</v>
+      </c>
+      <c r="J41" s="2">
+        <v>3</v>
+      </c>
+      <c r="K41" s="2">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>4</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1241,14 +2788,50 @@
       <c r="C42">
         <v>0</v>
       </c>
-      <c r="D42" s="1">
-        <v>2</v>
-      </c>
-      <c r="E42" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2">
+        <v>1</v>
+      </c>
+      <c r="K42" s="2">
+        <v>2</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1256,7 +2839,7 @@
         <v>43</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1264,8 +2847,44 @@
       <c r="E43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="1">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0</v>
+      </c>
+      <c r="J43" s="2">
+        <v>1</v>
+      </c>
+      <c r="K43" s="2">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>3</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1273,16 +2892,52 @@
         <v>44</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0</v>
+      </c>
+      <c r="J44" s="2">
+        <v>1</v>
+      </c>
+      <c r="K44" s="2">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>4</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1298,8 +2953,44 @@
       <c r="E45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2">
+        <v>1</v>
+      </c>
+      <c r="K45" s="2">
+        <v>3</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>4</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q45" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1310,13 +3001,49 @@
         <v>0</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2">
+        <v>1</v>
+      </c>
+      <c r="K46" s="2">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1324,16 +3051,52 @@
         <v>47</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="F47" s="1">
+        <v>4</v>
+      </c>
+      <c r="G47">
+        <v>3.5</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0</v>
+      </c>
+      <c r="J47" s="2">
+        <v>1</v>
+      </c>
+      <c r="K47" s="2">
+        <v>4</v>
+      </c>
+      <c r="L47">
+        <v>3</v>
+      </c>
+      <c r="M47">
+        <v>2</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1341,16 +3104,52 @@
         <v>48</v>
       </c>
       <c r="C48">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48">
+        <v>4</v>
+      </c>
+      <c r="I48" s="2">
+        <v>4</v>
+      </c>
+      <c r="J48" s="2">
+        <v>0</v>
+      </c>
+      <c r="K48" s="2">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>4</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>5</v>
+      </c>
+      <c r="P48" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1358,16 +3157,52 @@
         <v>49</v>
       </c>
       <c r="C49">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49" s="2">
+        <v>3</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0</v>
+      </c>
+      <c r="K49" s="2">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>2</v>
+      </c>
+      <c r="P49" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1375,7 +3210,7 @@
         <v>50</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -1383,8 +3218,44 @@
       <c r="E50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="1">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>5</v>
+      </c>
+      <c r="I50" s="2">
+        <v>1</v>
+      </c>
+      <c r="J50" s="2">
+        <v>5</v>
+      </c>
+      <c r="K50" s="2">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1392,16 +3263,52 @@
         <v>51</v>
       </c>
       <c r="C51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>3</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0</v>
+      </c>
+      <c r="J51" s="2">
+        <v>5</v>
+      </c>
+      <c r="K51" s="2">
+        <v>3</v>
+      </c>
+      <c r="L51">
+        <v>3</v>
+      </c>
+      <c r="M51">
+        <v>2</v>
+      </c>
+      <c r="N51">
+        <v>4</v>
+      </c>
+      <c r="O51">
+        <v>3.5</v>
+      </c>
+      <c r="P51" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1409,16 +3316,52 @@
         <v>52</v>
       </c>
       <c r="C52">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <v>5</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52" s="2">
+        <v>5</v>
+      </c>
+      <c r="J52" s="2">
+        <v>0</v>
+      </c>
+      <c r="K52" s="2">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>2</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>4</v>
+      </c>
+      <c r="P52" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1434,22 +3377,306 @@
       <c r="E53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="F53" s="1">
+        <v>4</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53" s="2">
+        <v>4</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0</v>
+      </c>
+      <c r="K53" s="2">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>2</v>
+      </c>
+      <c r="M53">
+        <v>4</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>5</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54">
+        <v>5</v>
+      </c>
+      <c r="H54">
+        <v>2.5</v>
+      </c>
+      <c r="I54" s="6">
+        <v>0</v>
+      </c>
+      <c r="J54" s="6">
+        <v>5</v>
+      </c>
+      <c r="K54" s="6">
+        <v>5</v>
+      </c>
+      <c r="L54" s="6">
+        <v>3</v>
+      </c>
+      <c r="M54" s="6">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="C54">
-        <v>3</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
+      <c r="B55" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55" s="6">
+        <v>0</v>
+      </c>
+      <c r="J55" s="6">
+        <v>5</v>
+      </c>
+      <c r="K55" s="6">
+        <v>5</v>
+      </c>
+      <c r="L55" s="6">
+        <v>3</v>
+      </c>
+      <c r="M55" s="6">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
+      <c r="P55" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>3</v>
+      </c>
+      <c r="I56" s="6">
+        <v>0</v>
+      </c>
+      <c r="J56" s="6">
+        <v>2</v>
+      </c>
+      <c r="K56" s="6">
+        <v>5</v>
+      </c>
+      <c r="L56" s="6">
+        <v>3</v>
+      </c>
+      <c r="M56" s="6">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
+      <c r="P56" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q56" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <v>4</v>
+      </c>
+      <c r="F57" s="1">
+        <v>5</v>
+      </c>
+      <c r="G57">
+        <v>5</v>
+      </c>
+      <c r="H57">
+        <v>5</v>
+      </c>
+      <c r="I57" s="6">
+        <v>5</v>
+      </c>
+      <c r="J57" s="6">
+        <v>3</v>
+      </c>
+      <c r="K57" s="6">
+        <v>5</v>
+      </c>
+      <c r="L57" s="6">
+        <v>4</v>
+      </c>
+      <c r="M57" s="6">
+        <v>5</v>
+      </c>
+      <c r="N57">
+        <v>3</v>
+      </c>
+      <c r="O57">
+        <v>1</v>
+      </c>
+      <c r="P57" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q57" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58">
+        <v>4</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>5</v>
+      </c>
+      <c r="I58" s="6">
+        <v>4</v>
+      </c>
+      <c r="J58" s="6">
+        <v>3</v>
+      </c>
+      <c r="K58" s="6">
+        <v>5</v>
+      </c>
+      <c r="L58" s="6">
+        <v>3</v>
+      </c>
+      <c r="M58" s="6">
+        <v>5</v>
+      </c>
+      <c r="N58">
+        <v>4</v>
+      </c>
+      <c r="O58">
+        <v>5</v>
+      </c>
+      <c r="P58">
+        <v>4</v>
+      </c>
+      <c r="Q58" s="4">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hybrid system error is fixed
</commit_message>
<xml_diff>
--- a/05180000017_Deniz_Yürekdeler_Project2/ActivityRecommender_PythonCode/Real-Data/Activity-Rating-Real-Data.xlsx
+++ b/05180000017_Deniz_Yürekdeler_Project2/ActivityRecommender_PythonCode/Real-Data/Activity-Rating-Real-Data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>activityId</t>
   </si>
@@ -239,13 +239,19 @@
     <t>Dogukan</t>
   </si>
   <si>
-    <t>Kaan</t>
-  </si>
-  <si>
     <t>KaanGircek</t>
   </si>
   <si>
     <t>Omer</t>
+  </si>
+  <si>
+    <t>Taner</t>
+  </si>
+  <si>
+    <t>Bergin</t>
+  </si>
+  <si>
+    <t>KaanSaglam</t>
   </si>
 </sst>
 </file>
@@ -296,7 +302,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -310,6 +316,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -605,7 +614,7 @@
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -640,7 +649,7 @@
         <v>65</v>
       </c>
       <c r="L1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="M1" t="s">
         <v>66</v>
@@ -652,13 +661,19 @@
         <v>67</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="S1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -710,8 +725,14 @@
       <c r="Q2" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" s="7">
+        <v>5</v>
+      </c>
+      <c r="S2" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>2</v>
       </c>
@@ -763,8 +784,14 @@
       <c r="Q3" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" s="7">
+        <v>5</v>
+      </c>
+      <c r="S3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>3</v>
       </c>
@@ -816,8 +843,14 @@
       <c r="Q4" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" s="7">
+        <v>4</v>
+      </c>
+      <c r="S4" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>4</v>
       </c>
@@ -869,8 +902,14 @@
       <c r="Q5" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5" s="7">
+        <v>5</v>
+      </c>
+      <c r="S5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>5</v>
       </c>
@@ -922,8 +961,14 @@
       <c r="Q6" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R6" s="7">
+        <v>5</v>
+      </c>
+      <c r="S6" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>6</v>
       </c>
@@ -975,8 +1020,14 @@
       <c r="Q7" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7" s="7">
+        <v>2</v>
+      </c>
+      <c r="S7" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1028,8 +1079,14 @@
       <c r="Q8" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8" s="7">
+        <v>3</v>
+      </c>
+      <c r="S8" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1081,8 +1138,14 @@
       <c r="Q9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9" s="7">
+        <v>3</v>
+      </c>
+      <c r="S9" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1134,8 +1197,14 @@
       <c r="Q10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="R10" s="7">
+        <v>3</v>
+      </c>
+      <c r="S10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1187,8 +1256,14 @@
       <c r="Q11" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11" s="7">
+        <v>1</v>
+      </c>
+      <c r="S11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1240,8 +1315,14 @@
       <c r="Q12" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R12" s="7">
+        <v>3</v>
+      </c>
+      <c r="S12" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1293,8 +1374,14 @@
       <c r="Q13" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13" s="7">
+        <v>5</v>
+      </c>
+      <c r="S13" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1346,8 +1433,14 @@
       <c r="Q14" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="R14" s="7">
+        <v>4</v>
+      </c>
+      <c r="S14" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1399,8 +1492,14 @@
       <c r="Q15" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15" s="7">
+        <v>4</v>
+      </c>
+      <c r="S15" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1452,8 +1551,14 @@
       <c r="Q16" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R16" s="7">
+        <v>3</v>
+      </c>
+      <c r="S16" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1505,8 +1610,14 @@
       <c r="Q17" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="R17" s="7">
+        <v>2</v>
+      </c>
+      <c r="S17" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1558,8 +1669,14 @@
       <c r="Q18" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="R18" s="7">
+        <v>5</v>
+      </c>
+      <c r="S18" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1611,8 +1728,14 @@
       <c r="Q19" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="R19" s="7">
+        <v>5</v>
+      </c>
+      <c r="S19" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1664,8 +1787,14 @@
       <c r="Q20" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="R20" s="7">
+        <v>3</v>
+      </c>
+      <c r="S20" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1717,8 +1846,14 @@
       <c r="Q21" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="R21" s="7">
+        <v>3</v>
+      </c>
+      <c r="S21" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1770,8 +1905,14 @@
       <c r="Q22" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="R22" s="7">
+        <v>2</v>
+      </c>
+      <c r="S22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1823,8 +1964,14 @@
       <c r="Q23" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="R23" s="7">
+        <v>2</v>
+      </c>
+      <c r="S23" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1876,8 +2023,14 @@
       <c r="Q24" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="R24" s="7">
+        <v>3</v>
+      </c>
+      <c r="S24" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1929,8 +2082,14 @@
       <c r="Q25" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="R25" s="7">
+        <v>4</v>
+      </c>
+      <c r="S25" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1982,8 +2141,14 @@
       <c r="Q26" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="R26" s="7">
+        <v>5</v>
+      </c>
+      <c r="S26" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2035,8 +2200,14 @@
       <c r="Q27" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="R27" s="7">
+        <v>2</v>
+      </c>
+      <c r="S27" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2088,8 +2259,14 @@
       <c r="Q28" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="R28" s="7">
+        <v>2</v>
+      </c>
+      <c r="S28" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2141,8 +2318,14 @@
       <c r="Q29" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="R29" s="7">
+        <v>3</v>
+      </c>
+      <c r="S29" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2194,8 +2377,14 @@
       <c r="Q30" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:17">
+      <c r="R30" s="7">
+        <v>3</v>
+      </c>
+      <c r="S30" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2247,8 +2436,14 @@
       <c r="Q31" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="R31" s="7">
+        <v>5</v>
+      </c>
+      <c r="S31" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2300,8 +2495,14 @@
       <c r="Q32" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="R32" s="7">
+        <v>4</v>
+      </c>
+      <c r="S32" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2353,8 +2554,14 @@
       <c r="Q33" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:17">
+      <c r="R33" s="7">
+        <v>5</v>
+      </c>
+      <c r="S33" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2406,8 +2613,14 @@
       <c r="Q34" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:17">
+      <c r="R34" s="7">
+        <v>4</v>
+      </c>
+      <c r="S34" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2459,8 +2672,14 @@
       <c r="Q35" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:17">
+      <c r="R35" s="7">
+        <v>3</v>
+      </c>
+      <c r="S35" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2512,8 +2731,14 @@
       <c r="Q36" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:17">
+      <c r="R36" s="7">
+        <v>5</v>
+      </c>
+      <c r="S36" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2565,8 +2790,14 @@
       <c r="Q37" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:17">
+      <c r="R37" s="7">
+        <v>1</v>
+      </c>
+      <c r="S37" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2618,8 +2849,14 @@
       <c r="Q38" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:17">
+      <c r="R38" s="7">
+        <v>4</v>
+      </c>
+      <c r="S38" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2671,8 +2908,14 @@
       <c r="Q39" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:17">
+      <c r="R39" s="7">
+        <v>3</v>
+      </c>
+      <c r="S39" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2724,8 +2967,14 @@
       <c r="Q40" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:17">
+      <c r="R40" s="7">
+        <v>5</v>
+      </c>
+      <c r="S40" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2777,8 +3026,14 @@
       <c r="Q41" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:17">
+      <c r="R41" s="7">
+        <v>0</v>
+      </c>
+      <c r="S41" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2830,8 +3085,14 @@
       <c r="Q42" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:17">
+      <c r="R42" s="7">
+        <v>0</v>
+      </c>
+      <c r="S42" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2883,8 +3144,14 @@
       <c r="Q43" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:17">
+      <c r="R43" s="7">
+        <v>0</v>
+      </c>
+      <c r="S43" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2936,8 +3203,14 @@
       <c r="Q44" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:17">
+      <c r="R44" s="7">
+        <v>0</v>
+      </c>
+      <c r="S44" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2989,8 +3262,14 @@
       <c r="Q45" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:17">
+      <c r="R45" s="7">
+        <v>0</v>
+      </c>
+      <c r="S45" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3042,8 +3321,14 @@
       <c r="Q46" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:17">
+      <c r="R46" s="7">
+        <v>0</v>
+      </c>
+      <c r="S46" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3095,8 +3380,14 @@
       <c r="Q47" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:17">
+      <c r="R47" s="7">
+        <v>0</v>
+      </c>
+      <c r="S47" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3148,8 +3439,14 @@
       <c r="Q48" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:17">
+      <c r="R48" s="7">
+        <v>0</v>
+      </c>
+      <c r="S48" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3201,8 +3498,14 @@
       <c r="Q49" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:17">
+      <c r="R49" s="7">
+        <v>0</v>
+      </c>
+      <c r="S49" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3254,8 +3557,14 @@
       <c r="Q50" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:17">
+      <c r="R50" s="7">
+        <v>0</v>
+      </c>
+      <c r="S50" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3307,8 +3616,14 @@
       <c r="Q51" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:17">
+      <c r="R51" s="7">
+        <v>1</v>
+      </c>
+      <c r="S51" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3360,8 +3675,14 @@
       <c r="Q52" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:17">
+      <c r="R52" s="7">
+        <v>3</v>
+      </c>
+      <c r="S52" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3413,8 +3734,14 @@
       <c r="Q53" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:17">
+      <c r="R53" s="7">
+        <v>1</v>
+      </c>
+      <c r="S53" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3466,8 +3793,14 @@
       <c r="Q54" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:17">
+      <c r="R54" s="7">
+        <v>2</v>
+      </c>
+      <c r="S54" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3519,8 +3852,14 @@
       <c r="Q55" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:17">
+      <c r="R55" s="7">
+        <v>2</v>
+      </c>
+      <c r="S55" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3572,8 +3911,14 @@
       <c r="Q56" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:17">
+      <c r="R56" s="7">
+        <v>2</v>
+      </c>
+      <c r="S56" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3625,8 +3970,14 @@
       <c r="Q57" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:17">
+      <c r="R57" s="7">
+        <v>1</v>
+      </c>
+      <c r="S57" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3676,6 +4027,12 @@
         <v>4</v>
       </c>
       <c r="Q58" s="4">
+        <v>4</v>
+      </c>
+      <c r="R58" s="7">
+        <v>5</v>
+      </c>
+      <c r="S58" s="6">
         <v>4</v>
       </c>
     </row>

</xml_diff>